<commit_message>
Ajout et configuration de Diverses Ressources
</commit_message>
<xml_diff>
--- a/WIP/Avancement.xlsx
+++ b/WIP/Avancement.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{841D18F1-E45C-46DD-8B14-6013D8BD9B9C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3142D1A-47E8-49C2-B8A7-F892E79458B8}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14,7 +14,6 @@
     <sheet name="MapJohto" sheetId="5" r:id="rId4"/>
     <sheet name="MapHoenn" sheetId="6" r:id="rId5"/>
     <sheet name="MapSinnoh" sheetId="7" r:id="rId6"/>
-    <sheet name="Musiques" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="201">
   <si>
     <t>Blue</t>
   </si>
@@ -607,9 +606,6 @@
     <t>Ranger H/F</t>
   </si>
   <si>
-    <t>Triathlete H/F</t>
-  </si>
-  <si>
     <t>Scientifique H/F</t>
   </si>
   <si>
@@ -620,13 +616,25 @@
   </si>
   <si>
     <t>Vendeur Shop</t>
+  </si>
+  <si>
+    <t>Rocket Butch</t>
+  </si>
+  <si>
+    <t>Rocket Cassady</t>
+  </si>
+  <si>
+    <t>Triathlete Course H/F</t>
+  </si>
+  <si>
+    <t>Triathlete Velo H/F</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -656,15 +664,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -685,11 +686,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -728,13 +724,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -750,11 +745,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="3" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="3">
     <cellStyle name="Insatisfaisant" xfId="2" builtinId="27"/>
-    <cellStyle name="Neutre" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Satisfaisant" xfId="1" builtinId="26"/>
   </cellStyles>
@@ -1037,7 +1030,7 @@
   <dimension ref="A1:O66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M33" sqref="M33"/>
+      <selection activeCell="N3" sqref="N3:O46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1117,21 +1110,21 @@
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3">
-        <v>1</v>
+      <c r="B3" s="4">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="3">
-        <v>1</v>
-      </c>
-      <c r="G3" s="3">
-        <v>1</v>
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="2" t="s">
@@ -1140,18 +1133,18 @@
       <c r="J3" s="4">
         <v>0</v>
       </c>
-      <c r="K3" s="3">
-        <v>1</v>
+      <c r="K3" s="4">
+        <v>0</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="N3" s="3">
-        <v>1</v>
-      </c>
-      <c r="O3" s="3">
-        <v>1</v>
+      <c r="N3" s="4">
+        <v>0</v>
+      </c>
+      <c r="O3" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -1161,18 +1154,18 @@
       <c r="B4" s="4">
         <v>0</v>
       </c>
-      <c r="C4" s="3">
-        <v>1</v>
+      <c r="C4" s="4">
+        <v>0</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="3">
-        <v>1</v>
-      </c>
-      <c r="G4" s="3">
-        <v>1</v>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="2" t="s">
@@ -1181,39 +1174,39 @@
       <c r="J4" s="4">
         <v>0</v>
       </c>
-      <c r="K4" s="3">
-        <v>1</v>
+      <c r="K4" s="4">
+        <v>0</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="N4" s="3">
-        <v>1</v>
-      </c>
-      <c r="O4" s="3">
-        <v>1</v>
+      <c r="N4" s="4">
+        <v>0</v>
+      </c>
+      <c r="O4" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="3">
-        <v>1</v>
-      </c>
-      <c r="C5" s="3">
-        <v>1</v>
+      <c r="B5" s="4">
+        <v>0</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F5" s="3">
-        <v>1</v>
-      </c>
-      <c r="G5" s="3">
-        <v>1</v>
+      <c r="F5" s="4">
+        <v>0</v>
+      </c>
+      <c r="G5" s="4">
+        <v>0</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="2" t="s">
@@ -1222,18 +1215,18 @@
       <c r="J5" s="4">
         <v>0</v>
       </c>
-      <c r="K5" s="3">
-        <v>1</v>
+      <c r="K5" s="4">
+        <v>0</v>
       </c>
       <c r="L5" s="1"/>
       <c r="M5" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="N5" s="3">
-        <v>1</v>
-      </c>
-      <c r="O5" s="3">
-        <v>1</v>
+      <c r="N5" s="4">
+        <v>0</v>
+      </c>
+      <c r="O5" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -1250,8 +1243,8 @@
       <c r="E6" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="F6" s="3">
-        <v>1</v>
+      <c r="F6" s="4">
+        <v>0</v>
       </c>
       <c r="G6" s="4">
         <v>0</v>
@@ -1270,8 +1263,8 @@
       <c r="M6" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="N6" s="3">
-        <v>1</v>
+      <c r="N6" s="4">
+        <v>0</v>
       </c>
       <c r="O6" s="4">
         <v>0</v>
@@ -1291,11 +1284,11 @@
       <c r="E7" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="F7" s="3">
-        <v>1</v>
-      </c>
-      <c r="G7" s="3">
-        <v>1</v>
+      <c r="F7" s="4">
+        <v>0</v>
+      </c>
+      <c r="G7" s="4">
+        <v>0</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="2" t="s">
@@ -1304,26 +1297,26 @@
       <c r="J7" s="4">
         <v>0</v>
       </c>
-      <c r="K7" s="3">
-        <v>1</v>
+      <c r="K7" s="4">
+        <v>0</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="N7" s="3">
-        <v>1</v>
-      </c>
-      <c r="O7" s="3">
-        <v>1</v>
+      <c r="N7" s="4">
+        <v>0</v>
+      </c>
+      <c r="O7" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="B8" s="3">
-        <v>1</v>
+      <c r="B8" s="4">
+        <v>0</v>
       </c>
       <c r="C8" s="4">
         <v>0</v>
@@ -1332,11 +1325,11 @@
       <c r="E8" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="F8" s="3">
-        <v>1</v>
-      </c>
-      <c r="G8" s="3">
-        <v>1</v>
+      <c r="F8" s="4">
+        <v>0</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="2" t="s">
@@ -1345,26 +1338,26 @@
       <c r="J8" s="4">
         <v>0</v>
       </c>
-      <c r="K8" s="3">
-        <v>1</v>
+      <c r="K8" s="4">
+        <v>0</v>
       </c>
       <c r="L8" s="1"/>
       <c r="M8" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="N8" s="3">
-        <v>1</v>
-      </c>
-      <c r="O8" s="3">
-        <v>1</v>
+      <c r="N8" s="4">
+        <v>0</v>
+      </c>
+      <c r="O8" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B9" s="3">
-        <v>1</v>
+      <c r="B9" s="4">
+        <v>0</v>
       </c>
       <c r="C9" s="4">
         <v>0</v>
@@ -1373,11 +1366,11 @@
       <c r="E9" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="F9" s="3">
-        <v>1</v>
-      </c>
-      <c r="G9" s="3">
-        <v>1</v>
+      <c r="F9" s="4">
+        <v>0</v>
+      </c>
+      <c r="G9" s="4">
+        <v>0</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="2" t="s">
@@ -1386,18 +1379,18 @@
       <c r="J9" s="4">
         <v>0</v>
       </c>
-      <c r="K9" s="3">
-        <v>1</v>
+      <c r="K9" s="4">
+        <v>0</v>
       </c>
       <c r="L9" s="1"/>
       <c r="M9" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="N9" s="3">
-        <v>1</v>
-      </c>
-      <c r="O9" s="3">
-        <v>1</v>
+      <c r="N9" s="4">
+        <v>0</v>
+      </c>
+      <c r="O9" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -1414,11 +1407,11 @@
       <c r="E10" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="F10" s="3">
-        <v>1</v>
-      </c>
-      <c r="G10" s="3">
-        <v>1</v>
+      <c r="F10" s="4">
+        <v>0</v>
+      </c>
+      <c r="G10" s="4">
+        <v>0</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="2" t="s">
@@ -1427,26 +1420,26 @@
       <c r="J10" s="4">
         <v>0</v>
       </c>
-      <c r="K10" s="3">
-        <v>1</v>
+      <c r="K10" s="4">
+        <v>0</v>
       </c>
       <c r="L10" s="1"/>
       <c r="M10" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="N10" s="3">
-        <v>1</v>
-      </c>
-      <c r="O10" s="3">
-        <v>1</v>
+      <c r="N10" s="4">
+        <v>0</v>
+      </c>
+      <c r="O10" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="B11" s="3">
-        <v>1</v>
+      <c r="B11" s="4">
+        <v>0</v>
       </c>
       <c r="C11" s="4">
         <v>0</v>
@@ -1455,11 +1448,11 @@
       <c r="E11" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="F11" s="3">
-        <v>1</v>
-      </c>
-      <c r="G11" s="3">
-        <v>1</v>
+      <c r="F11" s="4">
+        <v>0</v>
+      </c>
+      <c r="G11" s="4">
+        <v>0</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="2" t="s">
@@ -1468,26 +1461,26 @@
       <c r="J11" s="4">
         <v>0</v>
       </c>
-      <c r="K11" s="3">
-        <v>1</v>
+      <c r="K11" s="4">
+        <v>0</v>
       </c>
       <c r="L11" s="1"/>
       <c r="M11" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="N11" s="3">
-        <v>1</v>
-      </c>
-      <c r="O11" s="3">
-        <v>1</v>
+      <c r="N11" s="4">
+        <v>0</v>
+      </c>
+      <c r="O11" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="B12" s="3">
-        <v>1</v>
+      <c r="B12" s="4">
+        <v>0</v>
       </c>
       <c r="C12" s="4">
         <v>0</v>
@@ -1496,11 +1489,11 @@
       <c r="E12" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="F12" s="3">
-        <v>1</v>
-      </c>
-      <c r="G12" s="3">
-        <v>1</v>
+      <c r="F12" s="4">
+        <v>0</v>
+      </c>
+      <c r="G12" s="4">
+        <v>0</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="2" t="s">
@@ -1509,26 +1502,26 @@
       <c r="J12" s="4">
         <v>0</v>
       </c>
-      <c r="K12" s="3">
-        <v>1</v>
+      <c r="K12" s="4">
+        <v>0</v>
       </c>
       <c r="L12" s="1"/>
       <c r="M12" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="N12" s="3">
-        <v>1</v>
-      </c>
-      <c r="O12" s="3">
-        <v>1</v>
+      <c r="N12" s="4">
+        <v>0</v>
+      </c>
+      <c r="O12" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="B13" s="3">
-        <v>1</v>
+      <c r="B13" s="4">
+        <v>0</v>
       </c>
       <c r="C13" s="4">
         <v>0</v>
@@ -1537,11 +1530,11 @@
       <c r="E13" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F13" s="3">
-        <v>1</v>
-      </c>
-      <c r="G13" s="3">
-        <v>1</v>
+      <c r="F13" s="4">
+        <v>0</v>
+      </c>
+      <c r="G13" s="4">
+        <v>0</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="2" t="s">
@@ -1550,39 +1543,39 @@
       <c r="J13" s="4">
         <v>0</v>
       </c>
-      <c r="K13" s="3">
-        <v>1</v>
+      <c r="K13" s="4">
+        <v>0</v>
       </c>
       <c r="L13" s="1"/>
       <c r="M13" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="N13" s="3">
-        <v>1</v>
-      </c>
-      <c r="O13" s="3">
-        <v>1</v>
+      <c r="N13" s="4">
+        <v>0</v>
+      </c>
+      <c r="O13" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B14" s="3">
-        <v>1</v>
-      </c>
-      <c r="C14" s="3">
-        <v>1</v>
+      <c r="B14" s="4">
+        <v>0</v>
+      </c>
+      <c r="C14" s="4">
+        <v>0</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F14" s="3">
-        <v>1</v>
-      </c>
-      <c r="G14" s="3">
-        <v>1</v>
+      <c r="F14" s="4">
+        <v>0</v>
+      </c>
+      <c r="G14" s="4">
+        <v>0</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="2" t="s">
@@ -1591,39 +1584,39 @@
       <c r="J14" s="4">
         <v>0</v>
       </c>
-      <c r="K14" s="3">
-        <v>1</v>
+      <c r="K14" s="4">
+        <v>0</v>
       </c>
       <c r="L14" s="1"/>
       <c r="M14" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="N14" s="3">
-        <v>1</v>
-      </c>
-      <c r="O14" s="3">
-        <v>1</v>
+      <c r="N14" s="4">
+        <v>0</v>
+      </c>
+      <c r="O14" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B15" s="3">
-        <v>1</v>
-      </c>
-      <c r="C15" s="3">
-        <v>1</v>
+      <c r="B15" s="4">
+        <v>0</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="F15" s="3">
-        <v>1</v>
-      </c>
-      <c r="G15" s="3">
-        <v>1</v>
+      <c r="F15" s="4">
+        <v>0</v>
+      </c>
+      <c r="G15" s="4">
+        <v>0</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="2" t="s">
@@ -1632,39 +1625,39 @@
       <c r="J15" s="4">
         <v>0</v>
       </c>
-      <c r="K15" s="3">
-        <v>1</v>
+      <c r="K15" s="4">
+        <v>0</v>
       </c>
       <c r="L15" s="1"/>
       <c r="M15" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="N15" s="3">
-        <v>1</v>
-      </c>
-      <c r="O15" s="3">
-        <v>1</v>
+      <c r="N15" s="4">
+        <v>0</v>
+      </c>
+      <c r="O15" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B16" s="3">
-        <v>1</v>
-      </c>
-      <c r="C16" s="3">
-        <v>1</v>
+      <c r="B16" s="4">
+        <v>0</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="F16" s="3">
-        <v>1</v>
-      </c>
-      <c r="G16" s="3">
-        <v>1</v>
+      <c r="F16" s="4">
+        <v>0</v>
+      </c>
+      <c r="G16" s="4">
+        <v>0</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="6" t="s">
@@ -1673,39 +1666,39 @@
       <c r="J16" s="4">
         <v>0</v>
       </c>
-      <c r="K16" s="3">
-        <v>1</v>
+      <c r="K16" s="4">
+        <v>0</v>
       </c>
       <c r="L16" s="1"/>
       <c r="M16" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="N16" s="3">
-        <v>1</v>
-      </c>
-      <c r="O16" s="3">
-        <v>1</v>
+      <c r="N16" s="4">
+        <v>0</v>
+      </c>
+      <c r="O16" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B17" s="3">
-        <v>1</v>
-      </c>
-      <c r="C17" s="3">
-        <v>1</v>
+      <c r="B17" s="4">
+        <v>0</v>
+      </c>
+      <c r="C17" s="4">
+        <v>0</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="F17" s="3">
-        <v>1</v>
-      </c>
-      <c r="G17" s="3">
-        <v>1</v>
+      <c r="F17" s="4">
+        <v>0</v>
+      </c>
+      <c r="G17" s="4">
+        <v>0</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="2" t="s">
@@ -1714,39 +1707,39 @@
       <c r="J17" s="4">
         <v>0</v>
       </c>
-      <c r="K17" s="3">
-        <v>1</v>
+      <c r="K17" s="4">
+        <v>0</v>
       </c>
       <c r="L17" s="1"/>
       <c r="M17" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="N17" s="3">
-        <v>1</v>
-      </c>
-      <c r="O17" s="3">
-        <v>1</v>
+      <c r="N17" s="4">
+        <v>0</v>
+      </c>
+      <c r="O17" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B18" s="3">
-        <v>1</v>
-      </c>
-      <c r="C18" s="3">
-        <v>1</v>
+      <c r="B18" s="4">
+        <v>0</v>
+      </c>
+      <c r="C18" s="4">
+        <v>0</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="3">
-        <v>1</v>
-      </c>
-      <c r="G18" s="3">
-        <v>1</v>
+      <c r="F18" s="4">
+        <v>0</v>
+      </c>
+      <c r="G18" s="4">
+        <v>0</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="2" t="s">
@@ -1755,39 +1748,39 @@
       <c r="J18" s="4">
         <v>0</v>
       </c>
-      <c r="K18" s="3">
-        <v>1</v>
+      <c r="K18" s="4">
+        <v>0</v>
       </c>
       <c r="L18" s="1"/>
       <c r="M18" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="N18" s="3">
-        <v>1</v>
-      </c>
-      <c r="O18" s="3">
-        <v>1</v>
+      <c r="N18" s="4">
+        <v>0</v>
+      </c>
+      <c r="O18" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="B19" s="3">
-        <v>1</v>
-      </c>
-      <c r="C19" s="3">
-        <v>1</v>
+      <c r="B19" s="4">
+        <v>0</v>
+      </c>
+      <c r="C19" s="4">
+        <v>0</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="3">
-        <v>1</v>
-      </c>
-      <c r="G19" s="3">
-        <v>1</v>
+      <c r="F19" s="4">
+        <v>0</v>
+      </c>
+      <c r="G19" s="4">
+        <v>0</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="2" t="s">
@@ -1796,39 +1789,39 @@
       <c r="J19" s="4">
         <v>0</v>
       </c>
-      <c r="K19" s="3">
-        <v>1</v>
+      <c r="K19" s="4">
+        <v>0</v>
       </c>
       <c r="L19" s="1"/>
       <c r="M19" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="N19" s="3">
-        <v>1</v>
-      </c>
-      <c r="O19" s="3">
-        <v>1</v>
+      <c r="N19" s="4">
+        <v>0</v>
+      </c>
+      <c r="O19" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B20" s="3">
-        <v>1</v>
-      </c>
-      <c r="C20" s="3">
-        <v>1</v>
+      <c r="B20" s="4">
+        <v>0</v>
+      </c>
+      <c r="C20" s="4">
+        <v>0</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="3">
-        <v>1</v>
-      </c>
-      <c r="G20" s="3">
-        <v>1</v>
+      <c r="F20" s="4">
+        <v>0</v>
+      </c>
+      <c r="G20" s="4">
+        <v>0</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="2" t="s">
@@ -1837,59 +1830,59 @@
       <c r="J20" s="4">
         <v>0</v>
       </c>
-      <c r="K20" s="3">
-        <v>1</v>
+      <c r="K20" s="4">
+        <v>0</v>
       </c>
       <c r="L20" s="1"/>
       <c r="M20" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="N20" s="3">
-        <v>1</v>
-      </c>
-      <c r="O20" s="3">
-        <v>1</v>
+      <c r="N20" s="4">
+        <v>0</v>
+      </c>
+      <c r="O20" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B21" s="3">
-        <v>1</v>
-      </c>
-      <c r="C21" s="3">
-        <v>1</v>
+      <c r="B21" s="4">
+        <v>0</v>
+      </c>
+      <c r="C21" s="4">
+        <v>0</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F21" s="3">
-        <v>1</v>
-      </c>
-      <c r="G21" s="3">
-        <v>1</v>
+      <c r="F21" s="4">
+        <v>0</v>
+      </c>
+      <c r="G21" s="4">
+        <v>0</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="J21" s="3">
-        <v>1</v>
-      </c>
-      <c r="K21" s="3">
-        <v>1</v>
+      <c r="J21" s="4">
+        <v>0</v>
+      </c>
+      <c r="K21" s="4">
+        <v>0</v>
       </c>
       <c r="L21" s="1"/>
       <c r="M21" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="N21" s="3">
-        <v>1</v>
-      </c>
-      <c r="O21" s="3">
-        <v>1</v>
+      <c r="N21" s="4">
+        <v>0</v>
+      </c>
+      <c r="O21" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -1899,18 +1892,18 @@
       <c r="B22" s="4">
         <v>0</v>
       </c>
-      <c r="C22" s="3">
-        <v>1</v>
+      <c r="C22" s="4">
+        <v>0</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F22" s="3">
-        <v>1</v>
-      </c>
-      <c r="G22" s="3">
-        <v>1</v>
+      <c r="F22" s="4">
+        <v>0</v>
+      </c>
+      <c r="G22" s="4">
+        <v>0</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="2" t="s">
@@ -1919,36 +1912,36 @@
       <c r="J22" s="4">
         <v>0</v>
       </c>
-      <c r="K22" s="3">
-        <v>1</v>
+      <c r="K22" s="4">
+        <v>0</v>
       </c>
       <c r="L22" s="1"/>
       <c r="M22" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="N22" s="3">
-        <v>1</v>
-      </c>
-      <c r="O22" s="3">
-        <v>1</v>
+      <c r="N22" s="4">
+        <v>0</v>
+      </c>
+      <c r="O22" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="B23" s="3">
-        <v>1</v>
-      </c>
-      <c r="C23" s="3">
-        <v>1</v>
+      <c r="B23" s="4">
+        <v>0</v>
+      </c>
+      <c r="C23" s="4">
+        <v>0</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F23" s="3">
-        <v>1</v>
+      <c r="F23" s="4">
+        <v>0</v>
       </c>
       <c r="G23" s="4">
         <v>0</v>
@@ -1960,18 +1953,18 @@
       <c r="J23" s="4">
         <v>0</v>
       </c>
-      <c r="K23" s="3">
-        <v>1</v>
+      <c r="K23" s="4">
+        <v>0</v>
       </c>
       <c r="L23" s="1"/>
       <c r="M23" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="N23" s="3">
-        <v>1</v>
-      </c>
-      <c r="O23" s="3">
-        <v>1</v>
+      <c r="N23" s="4">
+        <v>0</v>
+      </c>
+      <c r="O23" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -1981,15 +1974,15 @@
       <c r="B24" s="4">
         <v>0</v>
       </c>
-      <c r="C24" s="3">
-        <v>1</v>
+      <c r="C24" s="4">
+        <v>0</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F24" s="3">
-        <v>1</v>
+      <c r="F24" s="4">
+        <v>0</v>
       </c>
       <c r="G24" s="4">
         <v>0</v>
@@ -2001,8 +1994,8 @@
       <c r="J24" s="4">
         <v>0</v>
       </c>
-      <c r="K24" s="3">
-        <v>1</v>
+      <c r="K24" s="4">
+        <v>0</v>
       </c>
       <c r="L24" s="1"/>
       <c r="M24" s="2" t="s">
@@ -2019,21 +2012,21 @@
       <c r="A25" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="B25" s="3">
-        <v>1</v>
-      </c>
-      <c r="C25" s="3">
-        <v>1</v>
+      <c r="B25" s="4">
+        <v>0</v>
+      </c>
+      <c r="C25" s="4">
+        <v>0</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F25" s="3">
-        <v>1</v>
-      </c>
-      <c r="G25" s="3">
-        <v>1</v>
+      <c r="F25" s="4">
+        <v>0</v>
+      </c>
+      <c r="G25" s="4">
+        <v>0</v>
       </c>
       <c r="H25" s="1"/>
       <c r="I25" s="2" t="s">
@@ -2042,39 +2035,39 @@
       <c r="J25" s="4">
         <v>0</v>
       </c>
-      <c r="K25" s="3">
-        <v>1</v>
+      <c r="K25" s="4">
+        <v>0</v>
       </c>
       <c r="L25" s="1"/>
       <c r="M25" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="N25" s="3">
-        <v>1</v>
-      </c>
-      <c r="O25" s="3">
-        <v>1</v>
+      <c r="N25" s="4">
+        <v>0</v>
+      </c>
+      <c r="O25" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="3">
-        <v>1</v>
-      </c>
-      <c r="C26" s="3">
-        <v>1</v>
+      <c r="B26" s="4">
+        <v>0</v>
+      </c>
+      <c r="C26" s="4">
+        <v>0</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F26" s="3">
-        <v>1</v>
-      </c>
-      <c r="G26" s="3">
-        <v>1</v>
+      <c r="F26" s="4">
+        <v>0</v>
+      </c>
+      <c r="G26" s="4">
+        <v>0</v>
       </c>
       <c r="H26" s="1"/>
       <c r="I26" s="2" t="s">
@@ -2083,39 +2076,39 @@
       <c r="J26" s="4">
         <v>0</v>
       </c>
-      <c r="K26" s="3">
-        <v>1</v>
+      <c r="K26" s="4">
+        <v>0</v>
       </c>
       <c r="L26" s="1"/>
       <c r="M26" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="N26" s="3">
-        <v>1</v>
-      </c>
-      <c r="O26" s="3">
-        <v>1</v>
+      <c r="N26" s="4">
+        <v>0</v>
+      </c>
+      <c r="O26" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="3">
-        <v>1</v>
-      </c>
-      <c r="C27" s="3">
-        <v>1</v>
+      <c r="B27" s="4">
+        <v>0</v>
+      </c>
+      <c r="C27" s="4">
+        <v>0</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="F27" s="3">
-        <v>1</v>
-      </c>
-      <c r="G27" s="3">
-        <v>1</v>
+      <c r="F27" s="4">
+        <v>0</v>
+      </c>
+      <c r="G27" s="4">
+        <v>0</v>
       </c>
       <c r="H27" s="1"/>
       <c r="I27" s="2" t="s">
@@ -2124,18 +2117,18 @@
       <c r="J27" s="4">
         <v>0</v>
       </c>
-      <c r="K27" s="3">
-        <v>1</v>
+      <c r="K27" s="4">
+        <v>0</v>
       </c>
       <c r="L27" s="1"/>
       <c r="M27" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="N27" s="3">
-        <v>1</v>
-      </c>
-      <c r="O27" s="3">
-        <v>1</v>
+      <c r="N27" s="4">
+        <v>0</v>
+      </c>
+      <c r="O27" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
@@ -2152,11 +2145,11 @@
       <c r="E28" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F28" s="3">
-        <v>1</v>
-      </c>
-      <c r="G28" s="3">
-        <v>1</v>
+      <c r="F28" s="4">
+        <v>0</v>
+      </c>
+      <c r="G28" s="4">
+        <v>0</v>
       </c>
       <c r="H28" s="1"/>
       <c r="I28" s="2" t="s">
@@ -2165,18 +2158,18 @@
       <c r="J28" s="4">
         <v>0</v>
       </c>
-      <c r="K28" s="3">
-        <v>1</v>
+      <c r="K28" s="4">
+        <v>0</v>
       </c>
       <c r="L28" s="1"/>
       <c r="M28" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="N28" s="3">
-        <v>1</v>
-      </c>
-      <c r="O28" s="3">
-        <v>1</v>
+      <c r="N28" s="4">
+        <v>0</v>
+      </c>
+      <c r="O28" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
@@ -2193,11 +2186,11 @@
       <c r="E29" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F29" s="3">
-        <v>1</v>
-      </c>
-      <c r="G29" s="3">
-        <v>1</v>
+      <c r="F29" s="4">
+        <v>0</v>
+      </c>
+      <c r="G29" s="4">
+        <v>0</v>
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="2" t="s">
@@ -2206,18 +2199,18 @@
       <c r="J29" s="4">
         <v>0</v>
       </c>
-      <c r="K29" s="3">
-        <v>1</v>
+      <c r="K29" s="4">
+        <v>0</v>
       </c>
       <c r="L29" s="1"/>
       <c r="M29" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="N29" s="3">
-        <v>1</v>
-      </c>
-      <c r="O29" s="3">
-        <v>1</v>
+      <c r="N29" s="4">
+        <v>0</v>
+      </c>
+      <c r="O29" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
@@ -2234,11 +2227,11 @@
       <c r="E30" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F30" s="3">
-        <v>1</v>
-      </c>
-      <c r="G30" s="3">
-        <v>1</v>
+      <c r="F30" s="4">
+        <v>0</v>
+      </c>
+      <c r="G30" s="4">
+        <v>0</v>
       </c>
       <c r="H30" s="1"/>
       <c r="I30" s="2" t="s">
@@ -2247,26 +2240,26 @@
       <c r="J30" s="4">
         <v>0</v>
       </c>
-      <c r="K30" s="3">
-        <v>1</v>
+      <c r="K30" s="4">
+        <v>0</v>
       </c>
       <c r="L30" s="1"/>
       <c r="M30" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="N30" s="3">
-        <v>1</v>
-      </c>
-      <c r="O30" s="3">
-        <v>1</v>
+      <c r="N30" s="4">
+        <v>0</v>
+      </c>
+      <c r="O30" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="B31" s="3">
-        <v>1</v>
+      <c r="A31" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="B31" s="4">
+        <v>0</v>
       </c>
       <c r="C31" s="4">
         <v>0</v>
@@ -2275,11 +2268,11 @@
       <c r="E31" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F31" s="3">
-        <v>1</v>
-      </c>
-      <c r="G31" s="3">
-        <v>1</v>
+      <c r="F31" s="4">
+        <v>0</v>
+      </c>
+      <c r="G31" s="4">
+        <v>0</v>
       </c>
       <c r="H31" s="1"/>
       <c r="I31" s="2" t="s">
@@ -2288,26 +2281,26 @@
       <c r="J31" s="4">
         <v>0</v>
       </c>
-      <c r="K31" s="3">
-        <v>1</v>
+      <c r="K31" s="4">
+        <v>0</v>
       </c>
       <c r="L31" s="1"/>
       <c r="M31" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="N31" s="3">
-        <v>1</v>
-      </c>
-      <c r="O31" s="3">
-        <v>1</v>
+      <c r="N31" s="4">
+        <v>0</v>
+      </c>
+      <c r="O31" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="B32" s="3">
-        <v>1</v>
+      <c r="A32" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="B32" s="4">
+        <v>0</v>
       </c>
       <c r="C32" s="4">
         <v>0</v>
@@ -2316,11 +2309,11 @@
       <c r="E32" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="F32" s="3">
-        <v>1</v>
-      </c>
-      <c r="G32" s="3">
-        <v>1</v>
+      <c r="F32" s="4">
+        <v>0</v>
+      </c>
+      <c r="G32" s="4">
+        <v>0</v>
       </c>
       <c r="H32" s="1"/>
       <c r="I32" s="2" t="s">
@@ -2329,8 +2322,8 @@
       <c r="J32" s="4">
         <v>0</v>
       </c>
-      <c r="K32" s="3">
-        <v>1</v>
+      <c r="K32" s="4">
+        <v>0</v>
       </c>
       <c r="L32" s="1"/>
       <c r="M32" s="2" t="s">
@@ -2345,23 +2338,23 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B33" s="3">
-        <v>1</v>
-      </c>
-      <c r="C33" s="3">
-        <v>1</v>
+        <v>195</v>
+      </c>
+      <c r="B33" s="4">
+        <v>0</v>
+      </c>
+      <c r="C33" s="4">
+        <v>0</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="F33" s="3">
-        <v>1</v>
-      </c>
-      <c r="G33" s="3">
-        <v>1</v>
+      <c r="F33" s="4">
+        <v>0</v>
+      </c>
+      <c r="G33" s="4">
+        <v>0</v>
       </c>
       <c r="H33" s="1"/>
       <c r="I33" s="2" t="s">
@@ -2370,29 +2363,29 @@
       <c r="J33" s="4">
         <v>0</v>
       </c>
-      <c r="K33" s="3">
-        <v>1</v>
+      <c r="K33" s="4">
+        <v>0</v>
       </c>
       <c r="L33" s="1"/>
       <c r="M33" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="N33" s="3">
-        <v>1</v>
-      </c>
-      <c r="O33" s="3">
-        <v>1</v>
+      <c r="N33" s="4">
+        <v>0</v>
+      </c>
+      <c r="O33" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>13</v>
+      <c r="A34" s="10" t="s">
+        <v>196</v>
       </c>
       <c r="B34" s="4">
         <v>0</v>
       </c>
-      <c r="C34" s="3">
-        <v>1</v>
+      <c r="C34" s="4">
+        <v>0</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="6"/>
@@ -2405,29 +2398,29 @@
       <c r="J34" s="4">
         <v>0</v>
       </c>
-      <c r="K34" s="3">
-        <v>1</v>
+      <c r="K34" s="4">
+        <v>0</v>
       </c>
       <c r="L34" s="1"/>
       <c r="M34" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="N34" s="3">
-        <v>1</v>
-      </c>
-      <c r="O34" s="3">
-        <v>1</v>
+      <c r="N34" s="4">
+        <v>0</v>
+      </c>
+      <c r="O34" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B35" s="3">
-        <v>1</v>
-      </c>
-      <c r="C35" s="3">
-        <v>1</v>
+        <v>12</v>
+      </c>
+      <c r="B35" s="4">
+        <v>0</v>
+      </c>
+      <c r="C35" s="4">
+        <v>0</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="6"/>
@@ -2440,29 +2433,29 @@
       <c r="J35" s="4">
         <v>0</v>
       </c>
-      <c r="K35" s="3">
-        <v>1</v>
+      <c r="K35" s="4">
+        <v>0</v>
       </c>
       <c r="L35" s="1"/>
       <c r="M35" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="N35" s="3">
-        <v>1</v>
-      </c>
-      <c r="O35" s="3">
-        <v>1</v>
+      <c r="N35" s="4">
+        <v>0</v>
+      </c>
+      <c r="O35" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B36" s="4">
         <v>0</v>
       </c>
-      <c r="C36" s="3">
-        <v>1</v>
+      <c r="C36" s="4">
+        <v>0</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="6"/>
@@ -2475,29 +2468,29 @@
       <c r="J36" s="4">
         <v>0</v>
       </c>
-      <c r="K36" s="3">
-        <v>1</v>
+      <c r="K36" s="4">
+        <v>0</v>
       </c>
       <c r="L36" s="1"/>
       <c r="M36" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="N36" s="3">
-        <v>1</v>
-      </c>
-      <c r="O36" s="3">
-        <v>1</v>
+      <c r="N36" s="4">
+        <v>0</v>
+      </c>
+      <c r="O36" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B37" s="3">
-        <v>1</v>
-      </c>
-      <c r="C37" s="3">
-        <v>1</v>
+        <v>14</v>
+      </c>
+      <c r="B37" s="4">
+        <v>0</v>
+      </c>
+      <c r="C37" s="4">
+        <v>0</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="6"/>
@@ -2510,29 +2503,29 @@
       <c r="J37" s="4">
         <v>0</v>
       </c>
-      <c r="K37" s="3">
-        <v>1</v>
+      <c r="K37" s="4">
+        <v>0</v>
       </c>
       <c r="L37" s="1"/>
       <c r="M37" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="N37" s="3">
-        <v>1</v>
-      </c>
-      <c r="O37" s="3">
-        <v>1</v>
+      <c r="N37" s="4">
+        <v>0</v>
+      </c>
+      <c r="O37" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B38" s="3">
-        <v>1</v>
-      </c>
-      <c r="C38" s="3">
-        <v>1</v>
+        <v>15</v>
+      </c>
+      <c r="B38" s="4">
+        <v>0</v>
+      </c>
+      <c r="C38" s="4">
+        <v>0</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="6"/>
@@ -2545,29 +2538,29 @@
       <c r="J38" s="4">
         <v>0</v>
       </c>
-      <c r="K38" s="3">
-        <v>1</v>
+      <c r="K38" s="4">
+        <v>0</v>
       </c>
       <c r="L38" s="1"/>
       <c r="M38" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="N38" s="3">
-        <v>1</v>
-      </c>
-      <c r="O38" s="3">
-        <v>1</v>
+      <c r="N38" s="4">
+        <v>0</v>
+      </c>
+      <c r="O38" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B39" s="3">
-        <v>1</v>
-      </c>
-      <c r="C39" s="3">
-        <v>1</v>
+        <v>16</v>
+      </c>
+      <c r="B39" s="4">
+        <v>0</v>
+      </c>
+      <c r="C39" s="4">
+        <v>0</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="2"/>
@@ -2580,15 +2573,15 @@
       <c r="J39" s="4">
         <v>0</v>
       </c>
-      <c r="K39" s="3">
-        <v>1</v>
+      <c r="K39" s="4">
+        <v>0</v>
       </c>
       <c r="L39" s="1"/>
       <c r="M39" s="10" t="s">
-        <v>195</v>
-      </c>
-      <c r="N39" s="3">
-        <v>1</v>
+        <v>194</v>
+      </c>
+      <c r="N39" s="4">
+        <v>0</v>
       </c>
       <c r="O39" s="4">
         <v>0</v>
@@ -2596,13 +2589,13 @@
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B40" s="3">
-        <v>1</v>
-      </c>
-      <c r="C40" s="3">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="B40" s="4">
+        <v>0</v>
+      </c>
+      <c r="C40" s="4">
+        <v>0</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="2"/>
@@ -2612,32 +2605,32 @@
       <c r="I40" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="J40" s="3">
-        <v>1</v>
-      </c>
-      <c r="K40" s="3">
-        <v>1</v>
+      <c r="J40" s="4">
+        <v>0</v>
+      </c>
+      <c r="K40" s="4">
+        <v>0</v>
       </c>
       <c r="L40" s="1"/>
       <c r="M40" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="N40" s="3">
-        <v>1</v>
-      </c>
-      <c r="O40" s="3">
-        <v>1</v>
+      <c r="N40" s="4">
+        <v>0</v>
+      </c>
+      <c r="O40" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B41" s="3">
-        <v>1</v>
-      </c>
-      <c r="C41" s="3">
-        <v>1</v>
+        <v>18</v>
+      </c>
+      <c r="B41" s="4">
+        <v>0</v>
+      </c>
+      <c r="C41" s="4">
+        <v>0</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="2"/>
@@ -2647,32 +2640,32 @@
       <c r="I41" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="J41" s="3">
-        <v>1</v>
-      </c>
-      <c r="K41" s="3">
-        <v>1</v>
+      <c r="J41" s="4">
+        <v>0</v>
+      </c>
+      <c r="K41" s="4">
+        <v>0</v>
       </c>
       <c r="L41" s="1"/>
       <c r="M41" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="N41" s="3">
-        <v>1</v>
-      </c>
-      <c r="O41" s="3">
-        <v>1</v>
+      <c r="N41" s="4">
+        <v>0</v>
+      </c>
+      <c r="O41" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B42" s="3">
-        <v>1</v>
-      </c>
-      <c r="C42" s="3">
-        <v>1</v>
+        <v>19</v>
+      </c>
+      <c r="B42" s="4">
+        <v>0</v>
+      </c>
+      <c r="C42" s="4">
+        <v>0</v>
       </c>
       <c r="D42" s="1"/>
       <c r="E42" s="2"/>
@@ -2685,29 +2678,29 @@
       <c r="J42" s="4">
         <v>0</v>
       </c>
-      <c r="K42" s="3">
-        <v>1</v>
+      <c r="K42" s="4">
+        <v>0</v>
       </c>
       <c r="L42" s="1"/>
       <c r="M42" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="N42" s="3">
-        <v>1</v>
-      </c>
-      <c r="O42" s="3">
-        <v>1</v>
+      <c r="N42" s="4">
+        <v>0</v>
+      </c>
+      <c r="O42" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B43" s="3">
-        <v>1</v>
-      </c>
-      <c r="C43" s="3">
-        <v>1</v>
+        <v>20</v>
+      </c>
+      <c r="B43" s="4">
+        <v>0</v>
+      </c>
+      <c r="C43" s="4">
+        <v>0</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="2"/>
@@ -2720,29 +2713,29 @@
       <c r="J43" s="4">
         <v>0</v>
       </c>
-      <c r="K43" s="3">
-        <v>1</v>
+      <c r="K43" s="4">
+        <v>0</v>
       </c>
       <c r="L43" s="1"/>
       <c r="M43" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="N43" s="11">
-        <v>0.5</v>
-      </c>
-      <c r="O43" s="3">
-        <v>1</v>
+      <c r="N43" s="4">
+        <v>0</v>
+      </c>
+      <c r="O43" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B44" s="3">
-        <v>1</v>
-      </c>
-      <c r="C44" s="3">
-        <v>1</v>
+        <v>21</v>
+      </c>
+      <c r="B44" s="4">
+        <v>0</v>
+      </c>
+      <c r="C44" s="4">
+        <v>0</v>
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="2"/>
@@ -2752,32 +2745,32 @@
       <c r="I44" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="J44" s="3">
-        <v>1</v>
-      </c>
-      <c r="K44" s="3">
-        <v>1</v>
+      <c r="J44" s="4">
+        <v>0</v>
+      </c>
+      <c r="K44" s="4">
+        <v>0</v>
       </c>
       <c r="L44" s="1"/>
       <c r="M44" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="N44" s="3">
-        <v>1</v>
-      </c>
-      <c r="O44" s="3">
-        <v>1</v>
+      <c r="N44" s="4">
+        <v>0</v>
+      </c>
+      <c r="O44" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B45" s="3">
-        <v>1</v>
-      </c>
-      <c r="C45" s="3">
-        <v>1</v>
+        <v>22</v>
+      </c>
+      <c r="B45" s="4">
+        <v>0</v>
+      </c>
+      <c r="C45" s="4">
+        <v>0</v>
       </c>
       <c r="D45" s="1"/>
       <c r="E45" s="2"/>
@@ -2790,29 +2783,29 @@
       <c r="J45" s="4">
         <v>0</v>
       </c>
-      <c r="K45" s="3">
-        <v>1</v>
+      <c r="K45" s="4">
+        <v>0</v>
       </c>
       <c r="L45" s="1"/>
       <c r="M45" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="N45" s="3">
-        <v>1</v>
-      </c>
-      <c r="O45" s="3">
-        <v>1</v>
+      <c r="N45" s="4">
+        <v>0</v>
+      </c>
+      <c r="O45" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B46" s="3">
-        <v>1</v>
-      </c>
-      <c r="C46" s="3">
-        <v>1</v>
+        <v>23</v>
+      </c>
+      <c r="B46" s="4">
+        <v>0</v>
+      </c>
+      <c r="C46" s="4">
+        <v>0</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="2"/>
@@ -2822,32 +2815,32 @@
       <c r="I46" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="J46" s="3">
-        <v>1</v>
-      </c>
-      <c r="K46" s="3">
-        <v>1</v>
+      <c r="J46" s="4">
+        <v>0</v>
+      </c>
+      <c r="K46" s="4">
+        <v>0</v>
       </c>
       <c r="L46" s="1"/>
       <c r="M46" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="N46" s="3">
-        <v>1</v>
-      </c>
-      <c r="O46" s="3">
-        <v>1</v>
+      <c r="N46" s="4">
+        <v>0</v>
+      </c>
+      <c r="O46" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="B47" s="3">
-        <v>1</v>
-      </c>
-      <c r="C47" s="3">
-        <v>1</v>
+        <v>24</v>
+      </c>
+      <c r="B47" s="4">
+        <v>0</v>
+      </c>
+      <c r="C47" s="4">
+        <v>0</v>
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="2"/>
@@ -2857,11 +2850,11 @@
       <c r="I47" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="J47" s="3">
-        <v>1</v>
-      </c>
-      <c r="K47" s="3">
-        <v>1</v>
+      <c r="J47" s="4">
+        <v>0</v>
+      </c>
+      <c r="K47" s="4">
+        <v>0</v>
       </c>
       <c r="L47" s="1"/>
       <c r="M47" s="2"/>
@@ -2870,13 +2863,13 @@
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="B48" s="3">
-        <v>1</v>
-      </c>
-      <c r="C48" s="3">
-        <v>1</v>
+        <v>25</v>
+      </c>
+      <c r="B48" s="4">
+        <v>0</v>
+      </c>
+      <c r="C48" s="4">
+        <v>0</v>
       </c>
       <c r="D48" s="1"/>
       <c r="E48" s="2"/>
@@ -2886,11 +2879,11 @@
       <c r="I48" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="J48" s="3">
-        <v>1</v>
-      </c>
-      <c r="K48" s="3">
-        <v>1</v>
+      <c r="J48" s="4">
+        <v>0</v>
+      </c>
+      <c r="K48" s="4">
+        <v>0</v>
       </c>
       <c r="L48" s="1"/>
       <c r="M48" s="2"/>
@@ -2898,14 +2891,14 @@
       <c r="O48" s="2"/>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A49" s="10" t="s">
-        <v>191</v>
-      </c>
-      <c r="B49" s="3">
-        <v>1</v>
-      </c>
-      <c r="C49" s="3">
-        <v>1</v>
+      <c r="A49" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B49" s="4">
+        <v>0</v>
+      </c>
+      <c r="C49" s="4">
+        <v>0</v>
       </c>
       <c r="D49" s="1"/>
       <c r="E49" s="2"/>
@@ -2915,11 +2908,11 @@
       <c r="I49" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="J49" s="3">
-        <v>1</v>
-      </c>
-      <c r="K49" s="3">
-        <v>1</v>
+      <c r="J49" s="4">
+        <v>0</v>
+      </c>
+      <c r="K49" s="4">
+        <v>0</v>
       </c>
       <c r="L49" s="1"/>
       <c r="M49" s="2"/>
@@ -2928,13 +2921,13 @@
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B50" s="3">
-        <v>1</v>
-      </c>
-      <c r="C50" s="3">
-        <v>1</v>
+        <v>177</v>
+      </c>
+      <c r="B50" s="4">
+        <v>0</v>
+      </c>
+      <c r="C50" s="4">
+        <v>0</v>
       </c>
       <c r="D50" s="1"/>
       <c r="E50" s="2"/>
@@ -2944,11 +2937,11 @@
       <c r="I50" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="J50" s="3">
-        <v>1</v>
-      </c>
-      <c r="K50" s="3">
-        <v>1</v>
+      <c r="J50" s="4">
+        <v>0</v>
+      </c>
+      <c r="K50" s="4">
+        <v>0</v>
       </c>
       <c r="L50" s="1"/>
       <c r="M50" s="2"/>
@@ -2956,14 +2949,14 @@
       <c r="O50" s="2"/>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B51" s="3">
-        <v>1</v>
-      </c>
-      <c r="C51" s="3">
-        <v>1</v>
+      <c r="A51" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="B51" s="4">
+        <v>0</v>
+      </c>
+      <c r="C51" s="4">
+        <v>0</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="2"/>
@@ -2973,11 +2966,11 @@
       <c r="I51" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="J51" s="3">
-        <v>1</v>
-      </c>
-      <c r="K51" s="3">
-        <v>1</v>
+      <c r="J51" s="4">
+        <v>0</v>
+      </c>
+      <c r="K51" s="4">
+        <v>0</v>
       </c>
       <c r="L51" s="1"/>
       <c r="M51" s="2"/>
@@ -2986,13 +2979,13 @@
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B52" s="3">
-        <v>1</v>
-      </c>
-      <c r="C52" s="3">
-        <v>1</v>
+        <v>26</v>
+      </c>
+      <c r="B52" s="4">
+        <v>0</v>
+      </c>
+      <c r="C52" s="4">
+        <v>0</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="2"/>
@@ -3005,8 +2998,8 @@
       <c r="J52" s="4">
         <v>0</v>
       </c>
-      <c r="K52" s="3">
-        <v>1</v>
+      <c r="K52" s="4">
+        <v>0</v>
       </c>
       <c r="L52" s="1"/>
       <c r="M52" s="2"/>
@@ -3014,14 +3007,14 @@
       <c r="O52" s="2"/>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A53" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B53" s="3">
-        <v>1</v>
-      </c>
-      <c r="C53" s="3">
-        <v>1</v>
+      <c r="A53" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B53" s="4">
+        <v>0</v>
+      </c>
+      <c r="C53" s="4">
+        <v>0</v>
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="2"/>
@@ -3031,11 +3024,11 @@
       <c r="I53" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="J53" s="3">
-        <v>1</v>
-      </c>
-      <c r="K53" s="3">
-        <v>1</v>
+      <c r="J53" s="4">
+        <v>0</v>
+      </c>
+      <c r="K53" s="4">
+        <v>0</v>
       </c>
       <c r="L53" s="1"/>
       <c r="M53" s="2"/>
@@ -3043,14 +3036,14 @@
       <c r="O53" s="2"/>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A54" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="B54" s="3">
-        <v>1</v>
-      </c>
-      <c r="C54" s="11">
-        <v>0.5</v>
+      <c r="A54" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B54" s="4">
+        <v>0</v>
+      </c>
+      <c r="C54" s="4">
+        <v>0</v>
       </c>
       <c r="D54" s="1"/>
       <c r="E54" s="2"/>
@@ -3060,11 +3053,11 @@
       <c r="I54" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="J54" s="3">
-        <v>1</v>
-      </c>
-      <c r="K54" s="3">
-        <v>1</v>
+      <c r="J54" s="4">
+        <v>0</v>
+      </c>
+      <c r="K54" s="4">
+        <v>0</v>
       </c>
       <c r="L54" s="1"/>
       <c r="M54" s="2"/>
@@ -3073,13 +3066,13 @@
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B55" s="3">
-        <v>1</v>
-      </c>
-      <c r="C55" s="3">
-        <v>1</v>
+        <v>29</v>
+      </c>
+      <c r="B55" s="4">
+        <v>0</v>
+      </c>
+      <c r="C55" s="4">
+        <v>0</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="2"/>
@@ -3089,11 +3082,11 @@
       <c r="I55" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="J55" s="3">
-        <v>1</v>
-      </c>
-      <c r="K55" s="3">
-        <v>1</v>
+      <c r="J55" s="4">
+        <v>0</v>
+      </c>
+      <c r="K55" s="4">
+        <v>0</v>
       </c>
       <c r="L55" s="1"/>
       <c r="M55" s="2"/>
@@ -3101,14 +3094,14 @@
       <c r="O55" s="2"/>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="B56" s="11">
-        <v>0.5</v>
-      </c>
-      <c r="C56" s="3">
-        <v>1</v>
+      <c r="A56" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="B56" s="4">
+        <v>0</v>
+      </c>
+      <c r="C56" s="4">
+        <v>0</v>
       </c>
       <c r="D56" s="1"/>
       <c r="E56" s="2"/>
@@ -3118,11 +3111,11 @@
       <c r="I56" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="J56" s="3">
-        <v>1</v>
-      </c>
-      <c r="K56" s="3">
-        <v>1</v>
+      <c r="J56" s="4">
+        <v>0</v>
+      </c>
+      <c r="K56" s="4">
+        <v>0</v>
       </c>
       <c r="L56" s="1"/>
       <c r="M56" s="2"/>
@@ -3131,13 +3124,13 @@
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="B57" s="3">
-        <v>1</v>
-      </c>
-      <c r="C57" s="3">
-        <v>1</v>
+        <v>30</v>
+      </c>
+      <c r="B57" s="4">
+        <v>0</v>
+      </c>
+      <c r="C57" s="4">
+        <v>0</v>
       </c>
       <c r="D57" s="1"/>
       <c r="E57" s="2"/>
@@ -3145,13 +3138,13 @@
       <c r="G57" s="2"/>
       <c r="H57" s="1"/>
       <c r="I57" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="J57" s="11">
-        <v>0.75</v>
-      </c>
-      <c r="K57" s="3">
-        <v>1</v>
+        <v>199</v>
+      </c>
+      <c r="J57" s="4">
+        <v>0</v>
+      </c>
+      <c r="K57" s="4">
+        <v>0</v>
       </c>
       <c r="L57" s="1"/>
       <c r="M57" s="2"/>
@@ -3159,26 +3152,44 @@
       <c r="O57" s="2"/>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A58" s="2"/>
-      <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
+      <c r="A58" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B58" s="4">
+        <v>0</v>
+      </c>
+      <c r="C58" s="4">
+        <v>0</v>
+      </c>
       <c r="D58" s="1"/>
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
       <c r="G58" s="2"/>
       <c r="H58" s="1"/>
-      <c r="I58" s="2"/>
-      <c r="J58" s="2"/>
-      <c r="K58" s="2"/>
+      <c r="I58" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="J58" s="4">
+        <v>0</v>
+      </c>
+      <c r="K58" s="4">
+        <v>0</v>
+      </c>
       <c r="L58" s="1"/>
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
       <c r="O58" s="2"/>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A59" s="2"/>
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
+      <c r="A59" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="B59" s="4">
+        <v>0</v>
+      </c>
+      <c r="C59" s="4">
+        <v>0</v>
+      </c>
       <c r="D59" s="1"/>
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
@@ -3299,42 +3310,42 @@
         <v>83</v>
       </c>
       <c r="B66" s="2">
-        <f>SUM(B3:B57)/55*100</f>
-        <v>79.090909090909093</v>
+        <f>SUM(B3:B59)/55*100</f>
+        <v>0</v>
       </c>
       <c r="C66" s="2">
-        <f>SUM(C3:C57)/55*100</f>
-        <v>75.454545454545453</v>
+        <f>SUM(C3:C59)/55*100</f>
+        <v>0</v>
       </c>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
       <c r="F66" s="2">
         <f>SUM(F3:F33)/31*100</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G66" s="2">
         <f>SUM(G3:G33)/31*100</f>
-        <v>90.322580645161281</v>
+        <v>0</v>
       </c>
       <c r="H66" s="1"/>
       <c r="I66" s="1"/>
       <c r="J66" s="2">
-        <f>SUM(J3:J53)/55*100</f>
-        <v>20</v>
+        <f>SUM(J3:J58)/55*100</f>
+        <v>0</v>
       </c>
       <c r="K66" s="2">
-        <f>SUM(K3:K53)/55*100</f>
-        <v>90.909090909090907</v>
+        <f>SUM(K3:K58)/55*100</f>
+        <v>0</v>
       </c>
       <c r="L66" s="1"/>
       <c r="M66" s="1"/>
       <c r="N66" s="2">
         <f>SUM(N3:N46)/44*100</f>
-        <v>94.318181818181827</v>
+        <v>0</v>
       </c>
       <c r="O66" s="2">
         <f>SUM(O3:O46)/44*100</f>
-        <v>90.909090909090907</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3348,7 +3359,7 @@
   <dimension ref="A1:G496"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14810,16 +14821,4 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB995872-CF71-48DD-8AB6-10790CE1FFAA}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>